<commit_message>
Updated who the collabarator
</commit_message>
<xml_diff>
--- a/documentation/Proposal.xlsx
+++ b/documentation/Proposal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C57CA91-827D-4A09-8DFF-0FFF0CAB19A2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E62CEF-AD1A-4798-9216-03245E1D4D6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>Our device is suppose to use thermal cameras in each of the desired rooms to detect human heat signature to determine number of people in the room. The light sensor will determine if room light is on give the user the ability to shut it on and off through the app and effeciently control electrcity bills. Finally, the BME280 will be used to determine the room temperature for user comfort. All this info will be sent to a device and transmitted to the app</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>https://github.com/KogulB/CENG355Project</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
 doi: 10.1109/CCE.2016.7562634
 keywords: {infrared detectors;local area networks;scheduling;sensor fusion;transport protocols;smart meeting room scheduling and management system;ad-hoc support;utilization control;real-time occupancy detection;meeting room occupancy status detection;scheduling application;ease-of-implementation solution;PIR sensor fusion device;Ethernet connectivity;UDP;IP protocol;web application;Scheduling;Servers;Real-time systems;Software;IP networks;Microcontrollers;Sockets;meeting scheduling;room management;real-time occupancy detection;utilization control;ad-hoc meetings},
 URL: http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=7562634&amp;isnumber=7562597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference Services </t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,7 +553,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -585,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -617,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="232" x14ac:dyDescent="0.35">
@@ -625,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -760,7 +760,7 @@
       </c>
       <c r="H2" s="2" t="str">
         <f>DataEntry!B8</f>
-        <v>N/A</v>
+        <v xml:space="preserve">Conference Services </v>
       </c>
       <c r="I2" s="2" t="str">
         <f>DataEntry!B9</f>

</xml_diff>